<commit_message>
energieverbruik update en random fixes
</commit_message>
<xml_diff>
--- a/omloop planning copy.xlsx
+++ b/omloop planning copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VScode\busje-komt-zo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69F93E4-8927-4F5D-909B-B4299C2ED967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A636C5FC-86B7-4E28-B92C-362294BF9993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2368,7 +2368,7 @@
   <dimension ref="A1:K721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,7 +2599,7 @@
         <v>401</v>
       </c>
       <c r="H7">
-        <v>10.803599999999999</v>
+        <v>1.8036000000000001</v>
       </c>
       <c r="I7" s="2">
         <v>45106.271527777782</v>
@@ -2666,7 +2666,7 @@
         <v>401</v>
       </c>
       <c r="H9">
-        <v>10.86</v>
+        <v>10000.86</v>
       </c>
       <c r="I9" s="2">
         <v>45106.288888888892</v>
@@ -2867,7 +2867,7 @@
         <v>401</v>
       </c>
       <c r="H15">
-        <v>10.86</v>
+        <v>100.86</v>
       </c>
       <c r="I15" s="2">
         <v>45106.35833333333</v>
@@ -3100,7 +3100,7 @@
         <v>14</v>
       </c>
       <c r="H22">
-        <v>10.32</v>
+        <v>0.69</v>
       </c>
       <c r="I22" s="2">
         <v>45106.479861111111</v>
@@ -3735,7 +3735,7 @@
         <v>401</v>
       </c>
       <c r="H41">
-        <v>10.86</v>
+        <v>100000.86</v>
       </c>
       <c r="I41" s="2">
         <v>45106.754166666673</v>
@@ -26437,6 +26437,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100931431478CF5164F9F4426B07FCEC3C0" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="04af3a1d4f66cf43f76c3176d0feadf6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbd7ad12-3323-416c-89da-709eb039707f" xmlns:ns3="c4c90c3b-e0bd-4787-87d0-fc55f607185c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6b79c2f15acc46f6342802de4a071dd" ns2:_="" ns3:_="">
     <xsd:import namespace="dbd7ad12-3323-416c-89da-709eb039707f"/>
@@ -26647,16 +26656,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7567438-8C04-4FBA-BDB9-3461D59EC70C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26673,12 +26681,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>